<commit_message>
Change the function name to start with __
</commit_message>
<xml_diff>
--- a/src/OpenAPI.Cms.TestTools/example.xlsx
+++ b/src/OpenAPI.Cms.TestTools/example.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Github\Dans\ExcelPublisher_Public\src\OpenAPI.Cms.TestTools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D732E82C-5AD8-48CD-98BB-B6CD82E4C7E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3D25EC9-1FDC-4730-A512-0FFE1AA18BD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3FBA689E-433E-47A2-BF8D-0E49C193B40C}"/>
   </bookViews>
   <sheets>
     <sheet name="strategy" sheetId="1" r:id="rId1"/>
     <sheet name="publish_config" sheetId="2" r:id="rId2"/>
-    <sheet name="Fairs" sheetId="3" r:id="rId3"/>
+    <sheet name="HistoricalFairs" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="fair">strategy!$N$3:$O$100</definedName>
@@ -1180,8 +1180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95651A8A-155D-45A0-966C-D3DF6E72C384}">
   <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1195,11 +1195,11 @@
       </c>
       <c r="C1" t="b">
         <f ca="1">AND(D1&gt;TIME(9,30,0),D1&lt;TIME(15,0,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D1" s="1">
         <f ca="1">NOW()-TODAY()</f>
-        <v>0.63388506944465917</v>
+        <v>0.59569629629550036</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -1758,7 +1758,7 @@
       </c>
       <c r="F3" s="18" t="b">
         <f ca="1">is_trading</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3" s="12">
         <v>100</v>
@@ -1822,20 +1822,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1910EBD8-8D4B-408E-BE47-91E912664919}">
-  <dimension ref="A1:K784"/>
+  <dimension ref="A1:I784"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.6640625" style="22" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.6640625" style="21" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="8.88671875" style="9"/>
+    <col min="9" max="9" width="10" style="21" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="23" cm="1">
-        <f t="array" ref="A1:C784">_xll.P_LoadReport(1000, publish_config!B4,publish_config!H4,publish_config!I4)</f>
+        <f t="array" ref="A1:C784">_xll.__LoadReport(1000, publish_config!B4,publish_config!H4,publish_config!I4)</f>
         <v>44517.614746458334</v>
       </c>
       <c r="B1" s="24" t="str">

</xml_diff>